<commit_message>
fix & add on form NCR
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEVELOPMENT MAGANG CBI\DEVELOPMENT LATIHAN MAGANG\REPO-TEAM-LATIHAN\ncr-app-v2\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFA91EC-6839-4842-8C39-055CCBBCA635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54D6525-D890-4B9B-84A5-C89210C85D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{8E92DE4D-D607-438C-8F89-D5AC85D7C7DC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E92DE4D-D607-438C-8F89-D5AC85D7C7DC}"/>
   </bookViews>
   <sheets>
     <sheet name="5 Supplier" sheetId="1" r:id="rId1"/>
@@ -2456,7 +2456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="52">
   <si>
     <t>Form-QAS-INC-11 (Laporan Ketidaksesuaian)</t>
   </si>
@@ -2596,31 +2596,7 @@
     <t>Foto:</t>
   </si>
   <si>
-    <t>Sering</t>
-  </si>
-  <si>
-    <t>Berulang</t>
-  </si>
-  <si>
-    <t>Pertama kali</t>
-  </si>
-  <si>
     <t>Frekuensi Masalah</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>WH-C/WH-FG</t>
-  </si>
-  <si>
-    <t>Produksi 2</t>
-  </si>
-  <si>
-    <t>Produksi 1</t>
-  </si>
-  <si>
-    <t>Incoming</t>
   </si>
   <si>
     <t xml:space="preserve">Problem Terjadi </t>
@@ -2633,12 +2609,6 @@
   </si>
   <si>
     <t>Department /  Supplier</t>
-  </si>
-  <si>
-    <t>Potensi masalah</t>
-  </si>
-  <si>
-    <t>Masalah</t>
   </si>
   <si>
     <t>Hal</t>
@@ -3424,7 +3394,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3702,9 +3672,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3714,12 +3681,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="26" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3801,6 +3762,144 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3831,24 +3930,12 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3879,69 +3966,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3969,68 +3993,11 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5198,8 +5165,8 @@
   </sheetPr>
   <dimension ref="B1:AT89"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="X40" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="AI73" sqref="AI73:AM75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="25" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="25.05" customHeight="1"/>
@@ -5216,87 +5183,87 @@
   <sheetData>
     <row r="1" spans="2:46" ht="8.25" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:46" ht="25.05" customHeight="1">
-      <c r="B2" s="125"/>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="173" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" s="174"/>
-      <c r="L2" s="174"/>
-      <c r="M2" s="174"/>
-      <c r="N2" s="174"/>
-      <c r="O2" s="174"/>
-      <c r="P2" s="174"/>
-      <c r="Q2" s="174"/>
-      <c r="R2" s="174"/>
-      <c r="S2" s="174"/>
-      <c r="T2" s="174"/>
-      <c r="U2" s="174"/>
-      <c r="V2" s="174"/>
-      <c r="W2" s="174"/>
-      <c r="X2" s="174"/>
-      <c r="Y2" s="174"/>
-      <c r="Z2" s="174"/>
-      <c r="AA2" s="174"/>
-      <c r="AB2" s="175"/>
-      <c r="AC2" s="182" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD2" s="141"/>
-      <c r="AE2" s="141"/>
-      <c r="AF2" s="138"/>
-      <c r="AG2" s="138" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH2" s="138"/>
-      <c r="AI2" s="138"/>
-      <c r="AJ2" s="138"/>
-      <c r="AK2" s="139" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL2" s="140"/>
-      <c r="AM2" s="140"/>
-      <c r="AN2" s="141"/>
-      <c r="AO2" s="126" t="s">
+      <c r="B2" s="122"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="191" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="192"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192"/>
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="193"/>
+      <c r="AC2" s="139" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2" s="140"/>
+      <c r="AE2" s="140"/>
+      <c r="AF2" s="141"/>
+      <c r="AG2" s="141" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" s="141"/>
+      <c r="AI2" s="141"/>
+      <c r="AJ2" s="141"/>
+      <c r="AK2" s="179" t="s">
+        <v>48</v>
+      </c>
+      <c r="AL2" s="180"/>
+      <c r="AM2" s="180"/>
+      <c r="AN2" s="140"/>
+      <c r="AO2" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" s="127"/>
-      <c r="AQ2" s="127"/>
-      <c r="AR2" s="127"/>
-      <c r="AS2" s="127"/>
-      <c r="AT2" s="128"/>
+      <c r="AP2" s="170"/>
+      <c r="AQ2" s="170"/>
+      <c r="AR2" s="170"/>
+      <c r="AS2" s="170"/>
+      <c r="AT2" s="171"/>
     </row>
     <row r="3" spans="2:46" ht="25.05" customHeight="1">
       <c r="B3" s="14"/>
-      <c r="F3" s="120"/>
+      <c r="F3" s="117"/>
       <c r="G3" s="81"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="177"/>
-      <c r="L3" s="177"/>
-      <c r="M3" s="177"/>
-      <c r="N3" s="177"/>
-      <c r="O3" s="177"/>
-      <c r="P3" s="177"/>
-      <c r="Q3" s="177"/>
-      <c r="R3" s="177"/>
-      <c r="S3" s="177"/>
-      <c r="T3" s="177"/>
-      <c r="U3" s="177"/>
-      <c r="V3" s="177"/>
-      <c r="W3" s="177"/>
-      <c r="X3" s="177"/>
-      <c r="Y3" s="177"/>
-      <c r="Z3" s="177"/>
-      <c r="AA3" s="177"/>
-      <c r="AB3" s="178"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="194"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
+      <c r="N3" s="195"/>
+      <c r="O3" s="195"/>
+      <c r="P3" s="195"/>
+      <c r="Q3" s="195"/>
+      <c r="R3" s="195"/>
+      <c r="S3" s="195"/>
+      <c r="T3" s="195"/>
+      <c r="U3" s="195"/>
+      <c r="V3" s="195"/>
+      <c r="W3" s="195"/>
+      <c r="X3" s="195"/>
+      <c r="Y3" s="195"/>
+      <c r="Z3" s="195"/>
+      <c r="AA3" s="195"/>
+      <c r="AB3" s="196"/>
       <c r="AC3" s="41"/>
       <c r="AD3" s="41"/>
       <c r="AE3" s="41"/>
@@ -5309,197 +5276,197 @@
       <c r="AL3" s="49"/>
       <c r="AM3" s="49"/>
       <c r="AN3" s="48"/>
-      <c r="AO3" s="129"/>
-      <c r="AP3" s="130"/>
-      <c r="AQ3" s="130"/>
-      <c r="AR3" s="130"/>
-      <c r="AS3" s="130"/>
-      <c r="AT3" s="131"/>
+      <c r="AO3" s="172"/>
+      <c r="AP3" s="173"/>
+      <c r="AQ3" s="173"/>
+      <c r="AR3" s="173"/>
+      <c r="AS3" s="173"/>
+      <c r="AT3" s="174"/>
     </row>
     <row r="4" spans="2:46" ht="25.05" customHeight="1" thickBot="1">
       <c r="B4" s="14"/>
-      <c r="F4" s="120"/>
+      <c r="F4" s="117"/>
       <c r="G4" s="81"/>
-      <c r="H4" s="113"/>
-      <c r="I4" s="113"/>
-      <c r="J4" s="179"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="180"/>
-      <c r="M4" s="180"/>
-      <c r="N4" s="180"/>
-      <c r="O4" s="180"/>
-      <c r="P4" s="180"/>
-      <c r="Q4" s="180"/>
-      <c r="R4" s="180"/>
-      <c r="S4" s="180"/>
-      <c r="T4" s="180"/>
-      <c r="U4" s="180"/>
-      <c r="V4" s="180"/>
-      <c r="W4" s="180"/>
-      <c r="X4" s="180"/>
-      <c r="Y4" s="180"/>
-      <c r="Z4" s="180"/>
-      <c r="AA4" s="180"/>
-      <c r="AB4" s="181"/>
-      <c r="AC4" s="108"/>
-      <c r="AD4" s="108"/>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="116"/>
-      <c r="AH4" s="108"/>
-      <c r="AI4" s="108"/>
-      <c r="AJ4" s="115"/>
-      <c r="AK4" s="116"/>
-      <c r="AL4" s="108"/>
-      <c r="AM4" s="108"/>
-      <c r="AN4" s="115"/>
-      <c r="AO4" s="132" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP4" s="133"/>
-      <c r="AQ4" s="133"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="197"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198"/>
+      <c r="N4" s="198"/>
+      <c r="O4" s="198"/>
+      <c r="P4" s="198"/>
+      <c r="Q4" s="198"/>
+      <c r="R4" s="198"/>
+      <c r="S4" s="198"/>
+      <c r="T4" s="198"/>
+      <c r="U4" s="198"/>
+      <c r="V4" s="198"/>
+      <c r="W4" s="198"/>
+      <c r="X4" s="198"/>
+      <c r="Y4" s="198"/>
+      <c r="Z4" s="198"/>
+      <c r="AA4" s="198"/>
+      <c r="AB4" s="199"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="105"/>
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="105"/>
+      <c r="AG4" s="113"/>
+      <c r="AH4" s="105"/>
+      <c r="AI4" s="105"/>
+      <c r="AJ4" s="112"/>
+      <c r="AK4" s="113"/>
+      <c r="AL4" s="105"/>
+      <c r="AM4" s="105"/>
+      <c r="AN4" s="112"/>
+      <c r="AO4" s="175" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP4" s="176"/>
+      <c r="AQ4" s="176"/>
       <c r="AR4" s="32"/>
       <c r="AS4" s="32"/>
-      <c r="AT4" s="114"/>
+      <c r="AT4" s="111"/>
     </row>
     <row r="5" spans="2:46" ht="12" customHeight="1" thickTop="1">
       <c r="B5" s="14"/>
-      <c r="F5" s="120"/>
+      <c r="F5" s="117"/>
       <c r="G5" s="81"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="119"/>
-      <c r="K5" s="118"/>
-      <c r="L5" s="118"/>
-      <c r="M5" s="118"/>
-      <c r="N5" s="118"/>
-      <c r="O5" s="118"/>
-      <c r="P5" s="118"/>
-      <c r="Q5" s="118"/>
-      <c r="R5" s="118"/>
-      <c r="S5" s="118"/>
-      <c r="T5" s="118"/>
-      <c r="U5" s="118"/>
-      <c r="V5" s="118"/>
-      <c r="W5" s="118"/>
-      <c r="X5" s="118"/>
-      <c r="Y5" s="118"/>
-      <c r="Z5" s="118"/>
-      <c r="AA5" s="118"/>
-      <c r="AB5" s="117"/>
-      <c r="AC5" s="108"/>
-      <c r="AD5" s="108"/>
-      <c r="AE5" s="108"/>
-      <c r="AF5" s="108"/>
-      <c r="AG5" s="116"/>
-      <c r="AH5" s="108"/>
-      <c r="AI5" s="108"/>
-      <c r="AJ5" s="115"/>
-      <c r="AK5" s="116"/>
-      <c r="AL5" s="108"/>
-      <c r="AM5" s="108"/>
-      <c r="AN5" s="115"/>
-      <c r="AO5" s="132"/>
-      <c r="AP5" s="133"/>
-      <c r="AQ5" s="133"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
+      <c r="Q5" s="115"/>
+      <c r="R5" s="115"/>
+      <c r="S5" s="115"/>
+      <c r="T5" s="115"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="115"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
+      <c r="AA5" s="115"/>
+      <c r="AB5" s="114"/>
+      <c r="AC5" s="105"/>
+      <c r="AD5" s="105"/>
+      <c r="AE5" s="105"/>
+      <c r="AF5" s="105"/>
+      <c r="AG5" s="113"/>
+      <c r="AH5" s="105"/>
+      <c r="AI5" s="105"/>
+      <c r="AJ5" s="112"/>
+      <c r="AK5" s="113"/>
+      <c r="AL5" s="105"/>
+      <c r="AM5" s="105"/>
+      <c r="AN5" s="112"/>
+      <c r="AO5" s="175"/>
+      <c r="AP5" s="176"/>
+      <c r="AQ5" s="176"/>
       <c r="AR5" s="32"/>
       <c r="AS5" s="32"/>
-      <c r="AT5" s="114"/>
+      <c r="AT5" s="111"/>
     </row>
     <row r="6" spans="2:46" ht="25.05" customHeight="1">
       <c r="B6" s="14"/>
       <c r="F6" s="81"/>
       <c r="G6" s="81"/>
-      <c r="H6" s="113"/>
-      <c r="I6" s="113"/>
-      <c r="J6" s="112"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="96"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="95" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="95"/>
       <c r="N6" s="81"/>
       <c r="O6" s="81"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="96" t="s">
-        <v>55</v>
+      <c r="P6" s="108"/>
+      <c r="Q6" s="95" t="s">
+        <v>45</v>
       </c>
       <c r="S6" s="81"/>
       <c r="U6" s="81"/>
-      <c r="V6" s="110"/>
-      <c r="W6" s="96" t="s">
-        <v>54</v>
+      <c r="V6" s="107"/>
+      <c r="W6" s="95" t="s">
+        <v>44</v>
       </c>
       <c r="X6" s="81"/>
       <c r="Y6" s="81"/>
       <c r="Z6" s="81"/>
       <c r="AA6" s="81"/>
-      <c r="AB6" s="109"/>
-      <c r="AC6" s="108"/>
-      <c r="AD6" s="108"/>
-      <c r="AE6" s="108"/>
-      <c r="AF6" s="108"/>
-      <c r="AG6" s="107"/>
-      <c r="AH6" s="106"/>
-      <c r="AI6" s="106"/>
-      <c r="AJ6" s="105"/>
-      <c r="AK6" s="107"/>
-      <c r="AL6" s="106"/>
-      <c r="AM6" s="106"/>
-      <c r="AN6" s="105"/>
-      <c r="AO6" s="142"/>
-      <c r="AP6" s="143"/>
-      <c r="AQ6" s="143"/>
-      <c r="AR6" s="143"/>
-      <c r="AS6" s="143"/>
-      <c r="AT6" s="144"/>
+      <c r="AB6" s="106"/>
+      <c r="AC6" s="105"/>
+      <c r="AD6" s="105"/>
+      <c r="AE6" s="105"/>
+      <c r="AF6" s="105"/>
+      <c r="AG6" s="104"/>
+      <c r="AH6" s="103"/>
+      <c r="AI6" s="103"/>
+      <c r="AJ6" s="102"/>
+      <c r="AK6" s="104"/>
+      <c r="AL6" s="103"/>
+      <c r="AM6" s="103"/>
+      <c r="AN6" s="102"/>
+      <c r="AO6" s="181"/>
+      <c r="AP6" s="182"/>
+      <c r="AQ6" s="182"/>
+      <c r="AR6" s="182"/>
+      <c r="AS6" s="182"/>
+      <c r="AT6" s="183"/>
     </row>
     <row r="7" spans="2:46" ht="25.05" customHeight="1" thickBot="1">
-      <c r="B7" s="104"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="100"/>
-      <c r="X7" s="100"/>
-      <c r="Y7" s="100"/>
-      <c r="Z7" s="100"/>
-      <c r="AA7" s="100"/>
-      <c r="AB7" s="99"/>
-      <c r="AC7" s="148"/>
-      <c r="AD7" s="148"/>
-      <c r="AE7" s="148"/>
-      <c r="AF7" s="148"/>
-      <c r="AG7" s="148"/>
-      <c r="AH7" s="148"/>
-      <c r="AI7" s="148"/>
-      <c r="AJ7" s="148"/>
-      <c r="AK7" s="148"/>
-      <c r="AL7" s="148"/>
-      <c r="AM7" s="148"/>
-      <c r="AN7" s="148"/>
-      <c r="AO7" s="145"/>
-      <c r="AP7" s="146"/>
-      <c r="AQ7" s="146"/>
-      <c r="AR7" s="146"/>
-      <c r="AS7" s="146"/>
-      <c r="AT7" s="147"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="100"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="97"/>
+      <c r="O7" s="97"/>
+      <c r="P7" s="97"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="97"/>
+      <c r="S7" s="97"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="97"/>
+      <c r="V7" s="97"/>
+      <c r="W7" s="97"/>
+      <c r="X7" s="97"/>
+      <c r="Y7" s="97"/>
+      <c r="Z7" s="97"/>
+      <c r="AA7" s="97"/>
+      <c r="AB7" s="96"/>
+      <c r="AC7" s="187"/>
+      <c r="AD7" s="187"/>
+      <c r="AE7" s="187"/>
+      <c r="AF7" s="187"/>
+      <c r="AG7" s="187"/>
+      <c r="AH7" s="187"/>
+      <c r="AI7" s="187"/>
+      <c r="AJ7" s="187"/>
+      <c r="AK7" s="187"/>
+      <c r="AL7" s="187"/>
+      <c r="AM7" s="187"/>
+      <c r="AN7" s="187"/>
+      <c r="AO7" s="184"/>
+      <c r="AP7" s="185"/>
+      <c r="AQ7" s="185"/>
+      <c r="AR7" s="185"/>
+      <c r="AS7" s="185"/>
+      <c r="AT7" s="186"/>
     </row>
     <row r="8" spans="2:46" ht="25.05" customHeight="1" thickTop="1">
       <c r="B8" s="14"/>
@@ -5587,28 +5554,24 @@
     <row r="11" spans="2:46" ht="25.05" customHeight="1">
       <c r="B11" s="14"/>
       <c r="C11" s="16"/>
-      <c r="D11" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96" t="s">
+      <c r="D11" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="95"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="95"/>
-      <c r="J11" s="94" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="98"/>
-      <c r="N11" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" s="94"/>
-      <c r="P11" s="94"/>
-      <c r="Q11" s="94"/>
+      <c r="I11"/>
+      <c r="J11" s="93"/>
+      <c r="K11" s="93"/>
+      <c r="L11" s="93"/>
+      <c r="M11"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="93"/>
       <c r="R11" s="92"/>
       <c r="S11" s="91"/>
       <c r="U11" s="16"/>
@@ -5641,24 +5604,24 @@
     <row r="12" spans="2:46" ht="25.05" customHeight="1">
       <c r="B12" s="14"/>
       <c r="C12" s="16"/>
-      <c r="D12" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96" t="s">
+      <c r="D12" s="95" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="95"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="95"/>
+      <c r="H12" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="94"/>
-      <c r="J12" s="94"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="94"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="94"/>
-      <c r="Q12" s="94"/>
+      <c r="I12" s="93"/>
+      <c r="J12" s="93"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="93"/>
+      <c r="M12" s="93"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="93"/>
       <c r="R12" s="92"/>
       <c r="S12" s="91"/>
       <c r="U12" s="16"/>
@@ -5689,24 +5652,24 @@
     <row r="13" spans="2:46" ht="25.05" customHeight="1">
       <c r="B13" s="14"/>
       <c r="C13" s="16"/>
-      <c r="D13" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96" t="s">
+      <c r="D13" s="95" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="95"/>
+      <c r="H13" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="94"/>
+      <c r="I13" s="93"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
+      <c r="M13" s="93"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="93"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="93"/>
       <c r="R13" s="92"/>
       <c r="S13" s="91"/>
       <c r="U13" s="16"/>
@@ -5739,24 +5702,24 @@
     <row r="14" spans="2:46" ht="25.05" customHeight="1">
       <c r="B14" s="14"/>
       <c r="C14" s="20"/>
-      <c r="D14" s="96" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="96"/>
-      <c r="F14" s="96"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96" t="s">
+      <c r="D14" s="95" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="95"/>
+      <c r="H14" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="94"/>
-      <c r="N14" s="94"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="94"/>
-      <c r="Q14" s="94"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="93"/>
+      <c r="L14" s="93"/>
+      <c r="M14" s="93"/>
+      <c r="N14" s="93"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="93"/>
       <c r="R14" s="92"/>
       <c r="S14" s="91"/>
       <c r="U14" s="11"/>
@@ -5789,31 +5752,25 @@
     <row r="15" spans="2:46" ht="25.05" customHeight="1">
       <c r="B15" s="14"/>
       <c r="C15" s="20"/>
-      <c r="D15" s="96" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="96" t="s">
+      <c r="D15" s="95" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="95"/>
-      <c r="J15" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="O15" s="94"/>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="95"/>
-      <c r="R15" s="92" t="s">
-        <v>44</v>
-      </c>
+      <c r="I15" s="200"/>
+      <c r="J15"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15"/>
+      <c r="R15" s="92"/>
       <c r="S15" s="91"/>
       <c r="Y15" s="32"/>
       <c r="Z15" s="32"/>
@@ -5825,24 +5782,20 @@
     <row r="16" spans="2:46" ht="25.05" customHeight="1">
       <c r="B16" s="14"/>
       <c r="C16" s="20"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="94" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="O16" s="94"/>
-      <c r="P16" s="94"/>
-      <c r="Q16" s="93"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="201"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16"/>
       <c r="R16" s="92"/>
       <c r="S16" s="91"/>
       <c r="U16" s="23"/>
@@ -5875,112 +5828,106 @@
     <row r="17" spans="2:46" ht="25.05" customHeight="1">
       <c r="B17" s="14"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="94"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="97"/>
-      <c r="N17" s="94"/>
-      <c r="O17" s="94"/>
-      <c r="P17" s="94"/>
-      <c r="Q17" s="97"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17"/>
+      <c r="J17" s="93"/>
+      <c r="K17" s="93"/>
+      <c r="L17" s="93"/>
+      <c r="M17"/>
+      <c r="N17" s="93"/>
+      <c r="O17" s="93"/>
+      <c r="P17" s="93"/>
+      <c r="Q17"/>
       <c r="R17" s="92"/>
       <c r="S17" s="91"/>
       <c r="U17" s="59"/>
-      <c r="V17" s="136" t="s">
+      <c r="V17" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="W17" s="152" t="s">
+      <c r="W17" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="X17" s="156"/>
-      <c r="Y17" s="156"/>
-      <c r="Z17" s="156"/>
-      <c r="AA17" s="156"/>
-      <c r="AB17" s="156"/>
-      <c r="AC17" s="156"/>
-      <c r="AD17" s="156"/>
-      <c r="AE17" s="156"/>
-      <c r="AF17" s="156"/>
-      <c r="AG17" s="156"/>
-      <c r="AH17" s="156"/>
-      <c r="AI17" s="156"/>
-      <c r="AJ17" s="153"/>
-      <c r="AK17" s="152" t="s">
+      <c r="X17" s="137"/>
+      <c r="Y17" s="137"/>
+      <c r="Z17" s="137"/>
+      <c r="AA17" s="137"/>
+      <c r="AB17" s="137"/>
+      <c r="AC17" s="137"/>
+      <c r="AD17" s="137"/>
+      <c r="AE17" s="137"/>
+      <c r="AF17" s="137"/>
+      <c r="AG17" s="137"/>
+      <c r="AH17" s="137"/>
+      <c r="AI17" s="137"/>
+      <c r="AJ17" s="134"/>
+      <c r="AK17" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="AL17" s="153"/>
-      <c r="AM17" s="152" t="s">
+      <c r="AL17" s="134"/>
+      <c r="AM17" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="AN17" s="156"/>
-      <c r="AO17" s="153"/>
-      <c r="AP17" s="158" t="s">
+      <c r="AN17" s="137"/>
+      <c r="AO17" s="134"/>
+      <c r="AP17" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="AQ17" s="159"/>
-      <c r="AR17" s="160"/>
+      <c r="AQ17" s="128"/>
+      <c r="AR17" s="129"/>
       <c r="AS17" s="58"/>
       <c r="AT17" s="8"/>
     </row>
     <row r="18" spans="2:46" ht="25.05" customHeight="1">
       <c r="B18" s="14"/>
       <c r="C18" s="20"/>
-      <c r="D18" s="96" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96" t="s">
+      <c r="D18" s="95" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="95"/>
-      <c r="J18" s="94" t="s">
-        <v>40</v>
-      </c>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="94" t="s">
-        <v>39</v>
-      </c>
-      <c r="O18" s="94"/>
-      <c r="P18" s="94"/>
-      <c r="Q18" s="93"/>
-      <c r="R18" s="92" t="s">
-        <v>38</v>
-      </c>
+      <c r="I18"/>
+      <c r="J18" s="93"/>
+      <c r="K18" s="93"/>
+      <c r="L18" s="93"/>
+      <c r="M18"/>
+      <c r="N18" s="93"/>
+      <c r="O18" s="93"/>
+      <c r="P18" s="93"/>
+      <c r="Q18"/>
+      <c r="R18" s="92"/>
       <c r="S18" s="91"/>
       <c r="U18" s="59"/>
-      <c r="V18" s="137"/>
-      <c r="W18" s="154"/>
-      <c r="X18" s="157"/>
-      <c r="Y18" s="157"/>
-      <c r="Z18" s="157"/>
-      <c r="AA18" s="157"/>
-      <c r="AB18" s="157"/>
-      <c r="AC18" s="157"/>
-      <c r="AD18" s="157"/>
-      <c r="AE18" s="157"/>
-      <c r="AF18" s="157"/>
-      <c r="AG18" s="157"/>
-      <c r="AH18" s="157"/>
-      <c r="AI18" s="157"/>
-      <c r="AJ18" s="155"/>
-      <c r="AK18" s="154"/>
-      <c r="AL18" s="155"/>
-      <c r="AM18" s="154"/>
-      <c r="AN18" s="157"/>
-      <c r="AO18" s="155"/>
-      <c r="AP18" s="161"/>
-      <c r="AQ18" s="162"/>
-      <c r="AR18" s="163"/>
+      <c r="V18" s="124"/>
+      <c r="W18" s="135"/>
+      <c r="X18" s="138"/>
+      <c r="Y18" s="138"/>
+      <c r="Z18" s="138"/>
+      <c r="AA18" s="138"/>
+      <c r="AB18" s="138"/>
+      <c r="AC18" s="138"/>
+      <c r="AD18" s="138"/>
+      <c r="AE18" s="138"/>
+      <c r="AF18" s="138"/>
+      <c r="AG18" s="138"/>
+      <c r="AH18" s="138"/>
+      <c r="AI18" s="138"/>
+      <c r="AJ18" s="136"/>
+      <c r="AK18" s="135"/>
+      <c r="AL18" s="136"/>
+      <c r="AM18" s="135"/>
+      <c r="AN18" s="138"/>
+      <c r="AO18" s="136"/>
+      <c r="AP18" s="130"/>
+      <c r="AQ18" s="131"/>
+      <c r="AR18" s="132"/>
       <c r="AS18" s="58"/>
       <c r="AT18" s="8"/>
     </row>
@@ -6005,20 +5952,20 @@
       <c r="S19" s="88"/>
       <c r="U19" s="59"/>
       <c r="V19" s="51"/>
-      <c r="W19" s="164"/>
-      <c r="X19" s="165"/>
-      <c r="Y19" s="165"/>
-      <c r="Z19" s="165"/>
-      <c r="AA19" s="165"/>
-      <c r="AB19" s="165"/>
-      <c r="AC19" s="165"/>
-      <c r="AD19" s="165"/>
-      <c r="AE19" s="165"/>
-      <c r="AF19" s="165"/>
-      <c r="AG19" s="165"/>
-      <c r="AH19" s="165"/>
-      <c r="AI19" s="165"/>
-      <c r="AJ19" s="166"/>
+      <c r="W19" s="154"/>
+      <c r="X19" s="155"/>
+      <c r="Y19" s="155"/>
+      <c r="Z19" s="155"/>
+      <c r="AA19" s="155"/>
+      <c r="AB19" s="155"/>
+      <c r="AC19" s="155"/>
+      <c r="AD19" s="155"/>
+      <c r="AE19" s="155"/>
+      <c r="AF19" s="155"/>
+      <c r="AG19" s="155"/>
+      <c r="AH19" s="155"/>
+      <c r="AI19" s="155"/>
+      <c r="AJ19" s="156"/>
       <c r="AK19" s="47"/>
       <c r="AL19" s="45"/>
       <c r="AM19" s="47"/>
@@ -6037,20 +5984,20 @@
       <c r="N20" s="2"/>
       <c r="U20" s="59"/>
       <c r="V20" s="43"/>
-      <c r="W20" s="167"/>
-      <c r="X20" s="168"/>
-      <c r="Y20" s="168"/>
-      <c r="Z20" s="168"/>
-      <c r="AA20" s="168"/>
-      <c r="AB20" s="168"/>
-      <c r="AC20" s="168"/>
-      <c r="AD20" s="168"/>
-      <c r="AE20" s="168"/>
-      <c r="AF20" s="168"/>
-      <c r="AG20" s="168"/>
-      <c r="AH20" s="168"/>
-      <c r="AI20" s="168"/>
-      <c r="AJ20" s="169"/>
+      <c r="W20" s="157"/>
+      <c r="X20" s="158"/>
+      <c r="Y20" s="158"/>
+      <c r="Z20" s="158"/>
+      <c r="AA20" s="158"/>
+      <c r="AB20" s="158"/>
+      <c r="AC20" s="158"/>
+      <c r="AD20" s="158"/>
+      <c r="AE20" s="158"/>
+      <c r="AF20" s="158"/>
+      <c r="AG20" s="158"/>
+      <c r="AH20" s="158"/>
+      <c r="AI20" s="158"/>
+      <c r="AJ20" s="159"/>
       <c r="AK20" s="39"/>
       <c r="AL20" s="38"/>
       <c r="AM20" s="39"/>
@@ -6085,20 +6032,20 @@
       <c r="S21" s="21"/>
       <c r="U21" s="59"/>
       <c r="V21" s="34"/>
-      <c r="W21" s="170"/>
-      <c r="X21" s="171"/>
-      <c r="Y21" s="171"/>
-      <c r="Z21" s="171"/>
-      <c r="AA21" s="171"/>
-      <c r="AB21" s="171"/>
-      <c r="AC21" s="171"/>
-      <c r="AD21" s="171"/>
-      <c r="AE21" s="171"/>
-      <c r="AF21" s="171"/>
-      <c r="AG21" s="171"/>
-      <c r="AH21" s="171"/>
-      <c r="AI21" s="171"/>
-      <c r="AJ21" s="172"/>
+      <c r="W21" s="160"/>
+      <c r="X21" s="161"/>
+      <c r="Y21" s="161"/>
+      <c r="Z21" s="161"/>
+      <c r="AA21" s="161"/>
+      <c r="AB21" s="161"/>
+      <c r="AC21" s="161"/>
+      <c r="AD21" s="161"/>
+      <c r="AE21" s="161"/>
+      <c r="AF21" s="161"/>
+      <c r="AG21" s="161"/>
+      <c r="AH21" s="161"/>
+      <c r="AI21" s="161"/>
+      <c r="AJ21" s="162"/>
       <c r="AK21" s="11"/>
       <c r="AL21" s="9"/>
       <c r="AM21" s="11"/>
@@ -6118,20 +6065,20 @@
       <c r="S22" s="15"/>
       <c r="U22" s="59"/>
       <c r="V22" s="36"/>
-      <c r="W22" s="195"/>
-      <c r="X22" s="196"/>
-      <c r="Y22" s="196"/>
-      <c r="Z22" s="196"/>
-      <c r="AA22" s="196"/>
-      <c r="AB22" s="196"/>
-      <c r="AC22" s="196"/>
-      <c r="AD22" s="196"/>
-      <c r="AE22" s="196"/>
-      <c r="AF22" s="196"/>
-      <c r="AG22" s="196"/>
-      <c r="AH22" s="196"/>
-      <c r="AI22" s="196"/>
-      <c r="AJ22" s="197"/>
+      <c r="W22" s="163"/>
+      <c r="X22" s="164"/>
+      <c r="Y22" s="164"/>
+      <c r="Z22" s="164"/>
+      <c r="AA22" s="164"/>
+      <c r="AB22" s="164"/>
+      <c r="AC22" s="164"/>
+      <c r="AD22" s="164"/>
+      <c r="AE22" s="164"/>
+      <c r="AF22" s="164"/>
+      <c r="AG22" s="164"/>
+      <c r="AH22" s="164"/>
+      <c r="AI22" s="164"/>
+      <c r="AJ22" s="165"/>
       <c r="AK22" s="23"/>
       <c r="AL22" s="21"/>
       <c r="AM22" s="23"/>
@@ -6151,20 +6098,20 @@
       <c r="S23" s="15"/>
       <c r="U23" s="59"/>
       <c r="V23" s="35"/>
-      <c r="W23" s="198"/>
-      <c r="X23" s="199"/>
-      <c r="Y23" s="199"/>
-      <c r="Z23" s="199"/>
-      <c r="AA23" s="199"/>
-      <c r="AB23" s="199"/>
-      <c r="AC23" s="199"/>
-      <c r="AD23" s="199"/>
-      <c r="AE23" s="199"/>
-      <c r="AF23" s="199"/>
-      <c r="AG23" s="199"/>
-      <c r="AH23" s="199"/>
-      <c r="AI23" s="199"/>
-      <c r="AJ23" s="200"/>
+      <c r="W23" s="166"/>
+      <c r="X23" s="167"/>
+      <c r="Y23" s="167"/>
+      <c r="Z23" s="167"/>
+      <c r="AA23" s="167"/>
+      <c r="AB23" s="167"/>
+      <c r="AC23" s="167"/>
+      <c r="AD23" s="167"/>
+      <c r="AE23" s="167"/>
+      <c r="AF23" s="167"/>
+      <c r="AG23" s="167"/>
+      <c r="AH23" s="167"/>
+      <c r="AI23" s="167"/>
+      <c r="AJ23" s="168"/>
       <c r="AK23" s="16"/>
       <c r="AL23" s="15"/>
       <c r="AM23" s="16"/>
@@ -6182,20 +6129,20 @@
       <c r="S24" s="15"/>
       <c r="U24" s="16"/>
       <c r="V24" s="34"/>
-      <c r="W24" s="192"/>
-      <c r="X24" s="193"/>
-      <c r="Y24" s="193"/>
-      <c r="Z24" s="193"/>
-      <c r="AA24" s="193"/>
-      <c r="AB24" s="193"/>
-      <c r="AC24" s="193"/>
-      <c r="AD24" s="193"/>
-      <c r="AE24" s="193"/>
-      <c r="AF24" s="193"/>
-      <c r="AG24" s="193"/>
-      <c r="AH24" s="193"/>
-      <c r="AI24" s="193"/>
-      <c r="AJ24" s="194"/>
+      <c r="W24" s="151"/>
+      <c r="X24" s="152"/>
+      <c r="Y24" s="152"/>
+      <c r="Z24" s="152"/>
+      <c r="AA24" s="152"/>
+      <c r="AB24" s="152"/>
+      <c r="AC24" s="152"/>
+      <c r="AD24" s="152"/>
+      <c r="AE24" s="152"/>
+      <c r="AF24" s="152"/>
+      <c r="AG24" s="152"/>
+      <c r="AH24" s="152"/>
+      <c r="AI24" s="152"/>
+      <c r="AJ24" s="153"/>
       <c r="AK24" s="11"/>
       <c r="AL24" s="9"/>
       <c r="AM24" s="11"/>
@@ -6298,39 +6245,39 @@
       <c r="N29" s="2"/>
       <c r="S29" s="15"/>
       <c r="U29" s="16"/>
-      <c r="V29" s="136" t="s">
+      <c r="V29" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="W29" s="152" t="s">
+      <c r="W29" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="X29" s="156"/>
-      <c r="Y29" s="156"/>
-      <c r="Z29" s="156"/>
-      <c r="AA29" s="156"/>
-      <c r="AB29" s="156"/>
-      <c r="AC29" s="156"/>
-      <c r="AD29" s="156"/>
-      <c r="AE29" s="156"/>
-      <c r="AF29" s="156"/>
-      <c r="AG29" s="156"/>
-      <c r="AH29" s="156"/>
-      <c r="AI29" s="156"/>
-      <c r="AJ29" s="153"/>
-      <c r="AK29" s="152" t="s">
+      <c r="X29" s="137"/>
+      <c r="Y29" s="137"/>
+      <c r="Z29" s="137"/>
+      <c r="AA29" s="137"/>
+      <c r="AB29" s="137"/>
+      <c r="AC29" s="137"/>
+      <c r="AD29" s="137"/>
+      <c r="AE29" s="137"/>
+      <c r="AF29" s="137"/>
+      <c r="AG29" s="137"/>
+      <c r="AH29" s="137"/>
+      <c r="AI29" s="137"/>
+      <c r="AJ29" s="134"/>
+      <c r="AK29" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="AL29" s="153"/>
-      <c r="AM29" s="152" t="s">
+      <c r="AL29" s="134"/>
+      <c r="AM29" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="AN29" s="156"/>
-      <c r="AO29" s="153"/>
-      <c r="AP29" s="158" t="s">
+      <c r="AN29" s="137"/>
+      <c r="AO29" s="134"/>
+      <c r="AP29" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="AQ29" s="159"/>
-      <c r="AR29" s="160"/>
+      <c r="AQ29" s="128"/>
+      <c r="AR29" s="129"/>
       <c r="AS29" s="37"/>
       <c r="AT29" s="8"/>
     </row>
@@ -6341,29 +6288,29 @@
       <c r="N30" s="2"/>
       <c r="S30" s="15"/>
       <c r="U30" s="16"/>
-      <c r="V30" s="137"/>
-      <c r="W30" s="154"/>
-      <c r="X30" s="157"/>
-      <c r="Y30" s="157"/>
-      <c r="Z30" s="157"/>
-      <c r="AA30" s="157"/>
-      <c r="AB30" s="157"/>
-      <c r="AC30" s="157"/>
-      <c r="AD30" s="157"/>
-      <c r="AE30" s="157"/>
-      <c r="AF30" s="157"/>
-      <c r="AG30" s="157"/>
-      <c r="AH30" s="157"/>
-      <c r="AI30" s="157"/>
-      <c r="AJ30" s="155"/>
-      <c r="AK30" s="154"/>
-      <c r="AL30" s="155"/>
-      <c r="AM30" s="154"/>
-      <c r="AN30" s="157"/>
-      <c r="AO30" s="155"/>
-      <c r="AP30" s="161"/>
-      <c r="AQ30" s="162"/>
-      <c r="AR30" s="163"/>
+      <c r="V30" s="124"/>
+      <c r="W30" s="135"/>
+      <c r="X30" s="138"/>
+      <c r="Y30" s="138"/>
+      <c r="Z30" s="138"/>
+      <c r="AA30" s="138"/>
+      <c r="AB30" s="138"/>
+      <c r="AC30" s="138"/>
+      <c r="AD30" s="138"/>
+      <c r="AE30" s="138"/>
+      <c r="AF30" s="138"/>
+      <c r="AG30" s="138"/>
+      <c r="AH30" s="138"/>
+      <c r="AI30" s="138"/>
+      <c r="AJ30" s="136"/>
+      <c r="AK30" s="135"/>
+      <c r="AL30" s="136"/>
+      <c r="AM30" s="135"/>
+      <c r="AN30" s="138"/>
+      <c r="AO30" s="136"/>
+      <c r="AP30" s="130"/>
+      <c r="AQ30" s="131"/>
+      <c r="AR30" s="132"/>
       <c r="AS30" s="37"/>
       <c r="AT30" s="8"/>
     </row>
@@ -6389,20 +6336,20 @@
       <c r="T31" s="1"/>
       <c r="U31" s="16"/>
       <c r="V31" s="51"/>
-      <c r="W31" s="164"/>
-      <c r="X31" s="165"/>
-      <c r="Y31" s="165"/>
-      <c r="Z31" s="165"/>
-      <c r="AA31" s="165"/>
-      <c r="AB31" s="165"/>
-      <c r="AC31" s="165"/>
-      <c r="AD31" s="165"/>
-      <c r="AE31" s="165"/>
-      <c r="AF31" s="165"/>
-      <c r="AG31" s="165"/>
-      <c r="AH31" s="165"/>
-      <c r="AI31" s="165"/>
-      <c r="AJ31" s="166"/>
+      <c r="W31" s="154"/>
+      <c r="X31" s="155"/>
+      <c r="Y31" s="155"/>
+      <c r="Z31" s="155"/>
+      <c r="AA31" s="155"/>
+      <c r="AB31" s="155"/>
+      <c r="AC31" s="155"/>
+      <c r="AD31" s="155"/>
+      <c r="AE31" s="155"/>
+      <c r="AF31" s="155"/>
+      <c r="AG31" s="155"/>
+      <c r="AH31" s="155"/>
+      <c r="AI31" s="155"/>
+      <c r="AJ31" s="156"/>
       <c r="AK31" s="47"/>
       <c r="AL31" s="45"/>
       <c r="AM31" s="47"/>
@@ -6422,20 +6369,20 @@
       <c r="S32" s="15"/>
       <c r="U32" s="16"/>
       <c r="V32" s="43"/>
-      <c r="W32" s="167"/>
-      <c r="X32" s="168"/>
-      <c r="Y32" s="168"/>
-      <c r="Z32" s="168"/>
-      <c r="AA32" s="168"/>
-      <c r="AB32" s="168"/>
-      <c r="AC32" s="168"/>
-      <c r="AD32" s="168"/>
-      <c r="AE32" s="168"/>
-      <c r="AF32" s="168"/>
-      <c r="AG32" s="168"/>
-      <c r="AH32" s="168"/>
-      <c r="AI32" s="168"/>
-      <c r="AJ32" s="169"/>
+      <c r="W32" s="157"/>
+      <c r="X32" s="158"/>
+      <c r="Y32" s="158"/>
+      <c r="Z32" s="158"/>
+      <c r="AA32" s="158"/>
+      <c r="AB32" s="158"/>
+      <c r="AC32" s="158"/>
+      <c r="AD32" s="158"/>
+      <c r="AE32" s="158"/>
+      <c r="AF32" s="158"/>
+      <c r="AG32" s="158"/>
+      <c r="AH32" s="158"/>
+      <c r="AI32" s="158"/>
+      <c r="AJ32" s="159"/>
       <c r="AK32" s="39"/>
       <c r="AL32" s="38"/>
       <c r="AM32" s="39"/>
@@ -6455,20 +6402,20 @@
       <c r="S33" s="15"/>
       <c r="U33" s="16"/>
       <c r="V33" s="34"/>
-      <c r="W33" s="170"/>
-      <c r="X33" s="171"/>
-      <c r="Y33" s="171"/>
-      <c r="Z33" s="171"/>
-      <c r="AA33" s="171"/>
-      <c r="AB33" s="171"/>
-      <c r="AC33" s="171"/>
-      <c r="AD33" s="171"/>
-      <c r="AE33" s="171"/>
-      <c r="AF33" s="171"/>
-      <c r="AG33" s="171"/>
-      <c r="AH33" s="171"/>
-      <c r="AI33" s="171"/>
-      <c r="AJ33" s="172"/>
+      <c r="W33" s="160"/>
+      <c r="X33" s="161"/>
+      <c r="Y33" s="161"/>
+      <c r="Z33" s="161"/>
+      <c r="AA33" s="161"/>
+      <c r="AB33" s="161"/>
+      <c r="AC33" s="161"/>
+      <c r="AD33" s="161"/>
+      <c r="AE33" s="161"/>
+      <c r="AF33" s="161"/>
+      <c r="AG33" s="161"/>
+      <c r="AH33" s="161"/>
+      <c r="AI33" s="161"/>
+      <c r="AJ33" s="162"/>
       <c r="AK33" s="11"/>
       <c r="AL33" s="9"/>
       <c r="AM33" s="11"/>
@@ -6488,20 +6435,20 @@
       <c r="S34" s="15"/>
       <c r="U34" s="16"/>
       <c r="V34" s="36"/>
-      <c r="W34" s="195"/>
-      <c r="X34" s="196"/>
-      <c r="Y34" s="196"/>
-      <c r="Z34" s="196"/>
-      <c r="AA34" s="196"/>
-      <c r="AB34" s="196"/>
-      <c r="AC34" s="196"/>
-      <c r="AD34" s="196"/>
-      <c r="AE34" s="196"/>
-      <c r="AF34" s="196"/>
-      <c r="AG34" s="196"/>
-      <c r="AH34" s="196"/>
-      <c r="AI34" s="196"/>
-      <c r="AJ34" s="197"/>
+      <c r="W34" s="163"/>
+      <c r="X34" s="164"/>
+      <c r="Y34" s="164"/>
+      <c r="Z34" s="164"/>
+      <c r="AA34" s="164"/>
+      <c r="AB34" s="164"/>
+      <c r="AC34" s="164"/>
+      <c r="AD34" s="164"/>
+      <c r="AE34" s="164"/>
+      <c r="AF34" s="164"/>
+      <c r="AG34" s="164"/>
+      <c r="AH34" s="164"/>
+      <c r="AI34" s="164"/>
+      <c r="AJ34" s="165"/>
       <c r="AK34" s="23"/>
       <c r="AL34" s="21"/>
       <c r="AM34" s="23"/>
@@ -6521,20 +6468,20 @@
       <c r="S35" s="15"/>
       <c r="U35" s="16"/>
       <c r="V35" s="35"/>
-      <c r="W35" s="198"/>
-      <c r="X35" s="199"/>
-      <c r="Y35" s="199"/>
-      <c r="Z35" s="199"/>
-      <c r="AA35" s="199"/>
-      <c r="AB35" s="199"/>
-      <c r="AC35" s="199"/>
-      <c r="AD35" s="199"/>
-      <c r="AE35" s="199"/>
-      <c r="AF35" s="199"/>
-      <c r="AG35" s="199"/>
-      <c r="AH35" s="199"/>
-      <c r="AI35" s="199"/>
-      <c r="AJ35" s="200"/>
+      <c r="W35" s="166"/>
+      <c r="X35" s="167"/>
+      <c r="Y35" s="167"/>
+      <c r="Z35" s="167"/>
+      <c r="AA35" s="167"/>
+      <c r="AB35" s="167"/>
+      <c r="AC35" s="167"/>
+      <c r="AD35" s="167"/>
+      <c r="AE35" s="167"/>
+      <c r="AF35" s="167"/>
+      <c r="AG35" s="167"/>
+      <c r="AH35" s="167"/>
+      <c r="AI35" s="167"/>
+      <c r="AJ35" s="168"/>
       <c r="AK35" s="16"/>
       <c r="AL35" s="15"/>
       <c r="AM35" s="16"/>
@@ -6552,20 +6499,20 @@
       <c r="S36" s="15"/>
       <c r="U36" s="16"/>
       <c r="V36" s="34"/>
-      <c r="W36" s="192"/>
-      <c r="X36" s="193"/>
-      <c r="Y36" s="193"/>
-      <c r="Z36" s="193"/>
-      <c r="AA36" s="193"/>
-      <c r="AB36" s="193"/>
-      <c r="AC36" s="193"/>
-      <c r="AD36" s="193"/>
-      <c r="AE36" s="193"/>
-      <c r="AF36" s="193"/>
-      <c r="AG36" s="193"/>
-      <c r="AH36" s="193"/>
-      <c r="AI36" s="193"/>
-      <c r="AJ36" s="194"/>
+      <c r="W36" s="151"/>
+      <c r="X36" s="152"/>
+      <c r="Y36" s="152"/>
+      <c r="Z36" s="152"/>
+      <c r="AA36" s="152"/>
+      <c r="AB36" s="152"/>
+      <c r="AC36" s="152"/>
+      <c r="AD36" s="152"/>
+      <c r="AE36" s="152"/>
+      <c r="AF36" s="152"/>
+      <c r="AG36" s="152"/>
+      <c r="AH36" s="152"/>
+      <c r="AI36" s="152"/>
+      <c r="AJ36" s="153"/>
       <c r="AK36" s="11"/>
       <c r="AL36" s="9"/>
       <c r="AM36" s="11"/>
@@ -6691,18 +6638,18 @@
       <c r="I40" s="22"/>
       <c r="J40" s="22"/>
       <c r="K40" s="21"/>
-      <c r="L40" s="149" t="s">
+      <c r="L40" s="188" t="s">
         <v>35</v>
       </c>
-      <c r="M40" s="150"/>
-      <c r="N40" s="150"/>
-      <c r="O40" s="151"/>
-      <c r="P40" s="149" t="s">
+      <c r="M40" s="189"/>
+      <c r="N40" s="189"/>
+      <c r="O40" s="190"/>
+      <c r="P40" s="188" t="s">
         <v>34</v>
       </c>
-      <c r="Q40" s="150"/>
-      <c r="R40" s="150"/>
-      <c r="S40" s="151"/>
+      <c r="Q40" s="189"/>
+      <c r="R40" s="189"/>
+      <c r="S40" s="190"/>
       <c r="U40" s="16"/>
       <c r="V40" s="47"/>
       <c r="W40" s="46"/>
@@ -6738,14 +6685,14 @@
       <c r="F41" s="73"/>
       <c r="G41" s="18"/>
       <c r="K41" s="15"/>
-      <c r="L41" s="134"/>
-      <c r="M41" s="134"/>
-      <c r="N41" s="134"/>
-      <c r="O41" s="134"/>
-      <c r="P41" s="134"/>
-      <c r="Q41" s="134"/>
-      <c r="R41" s="134"/>
-      <c r="S41" s="134"/>
+      <c r="L41" s="177"/>
+      <c r="M41" s="177"/>
+      <c r="N41" s="177"/>
+      <c r="O41" s="177"/>
+      <c r="P41" s="177"/>
+      <c r="Q41" s="177"/>
+      <c r="R41" s="177"/>
+      <c r="S41" s="177"/>
       <c r="U41" s="16"/>
       <c r="V41" s="39"/>
       <c r="W41" s="32"/>
@@ -6784,14 +6731,14 @@
       <c r="I42" s="79"/>
       <c r="J42" s="79"/>
       <c r="K42" s="82"/>
-      <c r="L42" s="135"/>
-      <c r="M42" s="135"/>
-      <c r="N42" s="135"/>
-      <c r="O42" s="135"/>
-      <c r="P42" s="135"/>
-      <c r="Q42" s="135"/>
-      <c r="R42" s="135"/>
-      <c r="S42" s="135"/>
+      <c r="L42" s="178"/>
+      <c r="M42" s="178"/>
+      <c r="N42" s="178"/>
+      <c r="O42" s="178"/>
+      <c r="P42" s="178"/>
+      <c r="Q42" s="178"/>
+      <c r="R42" s="178"/>
+      <c r="S42" s="178"/>
       <c r="U42" s="16"/>
       <c r="V42" s="16"/>
       <c r="Y42" s="32"/>
@@ -7003,39 +6950,39 @@
       <c r="R47" s="10"/>
       <c r="S47" s="9"/>
       <c r="U47" s="59"/>
-      <c r="V47" s="136" t="s">
+      <c r="V47" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="W47" s="152" t="s">
+      <c r="W47" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="X47" s="156"/>
-      <c r="Y47" s="156"/>
-      <c r="Z47" s="156"/>
-      <c r="AA47" s="156"/>
-      <c r="AB47" s="156"/>
-      <c r="AC47" s="156"/>
-      <c r="AD47" s="156"/>
-      <c r="AE47" s="156"/>
-      <c r="AF47" s="156"/>
-      <c r="AG47" s="156"/>
-      <c r="AH47" s="156"/>
-      <c r="AI47" s="156"/>
-      <c r="AJ47" s="153"/>
-      <c r="AK47" s="152" t="s">
+      <c r="X47" s="137"/>
+      <c r="Y47" s="137"/>
+      <c r="Z47" s="137"/>
+      <c r="AA47" s="137"/>
+      <c r="AB47" s="137"/>
+      <c r="AC47" s="137"/>
+      <c r="AD47" s="137"/>
+      <c r="AE47" s="137"/>
+      <c r="AF47" s="137"/>
+      <c r="AG47" s="137"/>
+      <c r="AH47" s="137"/>
+      <c r="AI47" s="137"/>
+      <c r="AJ47" s="134"/>
+      <c r="AK47" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="AL47" s="153"/>
-      <c r="AM47" s="152" t="s">
+      <c r="AL47" s="134"/>
+      <c r="AM47" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="AN47" s="156"/>
-      <c r="AO47" s="153"/>
-      <c r="AP47" s="158" t="s">
+      <c r="AN47" s="137"/>
+      <c r="AO47" s="134"/>
+      <c r="AP47" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="AQ47" s="159"/>
-      <c r="AR47" s="160"/>
+      <c r="AQ47" s="128"/>
+      <c r="AR47" s="129"/>
       <c r="AS47" s="58"/>
       <c r="AT47" s="8"/>
     </row>
@@ -7045,29 +6992,29 @@
       <c r="D48" s="17"/>
       <c r="N48" s="17"/>
       <c r="U48" s="59"/>
-      <c r="V48" s="137"/>
-      <c r="W48" s="154"/>
-      <c r="X48" s="157"/>
-      <c r="Y48" s="157"/>
-      <c r="Z48" s="157"/>
-      <c r="AA48" s="157"/>
-      <c r="AB48" s="157"/>
-      <c r="AC48" s="157"/>
-      <c r="AD48" s="157"/>
-      <c r="AE48" s="157"/>
-      <c r="AF48" s="157"/>
-      <c r="AG48" s="157"/>
-      <c r="AH48" s="157"/>
-      <c r="AI48" s="157"/>
-      <c r="AJ48" s="155"/>
-      <c r="AK48" s="154"/>
-      <c r="AL48" s="155"/>
-      <c r="AM48" s="154"/>
-      <c r="AN48" s="157"/>
-      <c r="AO48" s="155"/>
-      <c r="AP48" s="161"/>
-      <c r="AQ48" s="162"/>
-      <c r="AR48" s="163"/>
+      <c r="V48" s="124"/>
+      <c r="W48" s="135"/>
+      <c r="X48" s="138"/>
+      <c r="Y48" s="138"/>
+      <c r="Z48" s="138"/>
+      <c r="AA48" s="138"/>
+      <c r="AB48" s="138"/>
+      <c r="AC48" s="138"/>
+      <c r="AD48" s="138"/>
+      <c r="AE48" s="138"/>
+      <c r="AF48" s="138"/>
+      <c r="AG48" s="138"/>
+      <c r="AH48" s="138"/>
+      <c r="AI48" s="138"/>
+      <c r="AJ48" s="136"/>
+      <c r="AK48" s="135"/>
+      <c r="AL48" s="136"/>
+      <c r="AM48" s="135"/>
+      <c r="AN48" s="138"/>
+      <c r="AO48" s="136"/>
+      <c r="AP48" s="130"/>
+      <c r="AQ48" s="131"/>
+      <c r="AR48" s="132"/>
       <c r="AS48" s="58"/>
       <c r="AT48" s="8"/>
     </row>
@@ -7092,20 +7039,20 @@
       <c r="S49" s="21"/>
       <c r="U49" s="59"/>
       <c r="V49" s="51"/>
-      <c r="W49" s="164"/>
-      <c r="X49" s="165"/>
-      <c r="Y49" s="165"/>
-      <c r="Z49" s="165"/>
-      <c r="AA49" s="165"/>
-      <c r="AB49" s="165"/>
-      <c r="AC49" s="165"/>
-      <c r="AD49" s="165"/>
-      <c r="AE49" s="165"/>
-      <c r="AF49" s="165"/>
-      <c r="AG49" s="165"/>
-      <c r="AH49" s="165"/>
-      <c r="AI49" s="165"/>
-      <c r="AJ49" s="166"/>
+      <c r="W49" s="154"/>
+      <c r="X49" s="155"/>
+      <c r="Y49" s="155"/>
+      <c r="Z49" s="155"/>
+      <c r="AA49" s="155"/>
+      <c r="AB49" s="155"/>
+      <c r="AC49" s="155"/>
+      <c r="AD49" s="155"/>
+      <c r="AE49" s="155"/>
+      <c r="AF49" s="155"/>
+      <c r="AG49" s="155"/>
+      <c r="AH49" s="155"/>
+      <c r="AI49" s="155"/>
+      <c r="AJ49" s="156"/>
       <c r="AK49" s="47"/>
       <c r="AL49" s="45"/>
       <c r="AM49" s="47"/>
@@ -7142,20 +7089,20 @@
       <c r="S50" s="15"/>
       <c r="U50" s="59"/>
       <c r="V50" s="43"/>
-      <c r="W50" s="167"/>
-      <c r="X50" s="168"/>
-      <c r="Y50" s="168"/>
-      <c r="Z50" s="168"/>
-      <c r="AA50" s="168"/>
-      <c r="AB50" s="168"/>
-      <c r="AC50" s="168"/>
-      <c r="AD50" s="168"/>
-      <c r="AE50" s="168"/>
-      <c r="AF50" s="168"/>
-      <c r="AG50" s="168"/>
-      <c r="AH50" s="168"/>
-      <c r="AI50" s="168"/>
-      <c r="AJ50" s="169"/>
+      <c r="W50" s="157"/>
+      <c r="X50" s="158"/>
+      <c r="Y50" s="158"/>
+      <c r="Z50" s="158"/>
+      <c r="AA50" s="158"/>
+      <c r="AB50" s="158"/>
+      <c r="AC50" s="158"/>
+      <c r="AD50" s="158"/>
+      <c r="AE50" s="158"/>
+      <c r="AF50" s="158"/>
+      <c r="AG50" s="158"/>
+      <c r="AH50" s="158"/>
+      <c r="AI50" s="158"/>
+      <c r="AJ50" s="159"/>
       <c r="AK50" s="39"/>
       <c r="AL50" s="38"/>
       <c r="AM50" s="39"/>
@@ -7175,20 +7122,20 @@
       <c r="S51" s="15"/>
       <c r="U51" s="59"/>
       <c r="V51" s="34"/>
-      <c r="W51" s="170"/>
-      <c r="X51" s="171"/>
-      <c r="Y51" s="171"/>
-      <c r="Z51" s="171"/>
-      <c r="AA51" s="171"/>
-      <c r="AB51" s="171"/>
-      <c r="AC51" s="171"/>
-      <c r="AD51" s="171"/>
-      <c r="AE51" s="171"/>
-      <c r="AF51" s="171"/>
-      <c r="AG51" s="171"/>
-      <c r="AH51" s="171"/>
-      <c r="AI51" s="171"/>
-      <c r="AJ51" s="172"/>
+      <c r="W51" s="160"/>
+      <c r="X51" s="161"/>
+      <c r="Y51" s="161"/>
+      <c r="Z51" s="161"/>
+      <c r="AA51" s="161"/>
+      <c r="AB51" s="161"/>
+      <c r="AC51" s="161"/>
+      <c r="AD51" s="161"/>
+      <c r="AE51" s="161"/>
+      <c r="AF51" s="161"/>
+      <c r="AG51" s="161"/>
+      <c r="AH51" s="161"/>
+      <c r="AI51" s="161"/>
+      <c r="AJ51" s="162"/>
       <c r="AK51" s="11"/>
       <c r="AL51" s="9"/>
       <c r="AM51" s="11"/>
@@ -7205,34 +7152,34 @@
       <c r="C52" s="16"/>
       <c r="D52" s="61"/>
       <c r="E52" s="52"/>
-      <c r="F52" s="202"/>
-      <c r="G52" s="202"/>
-      <c r="H52" s="202"/>
-      <c r="I52" s="202"/>
+      <c r="F52" s="126"/>
+      <c r="G52" s="126"/>
+      <c r="H52" s="126"/>
+      <c r="I52" s="126"/>
       <c r="J52" s="52"/>
       <c r="K52" s="60"/>
       <c r="L52" s="52"/>
-      <c r="M52" s="202"/>
-      <c r="N52" s="202"/>
-      <c r="O52" s="202"/>
-      <c r="P52" s="202"/>
+      <c r="M52" s="126"/>
+      <c r="N52" s="126"/>
+      <c r="O52" s="126"/>
+      <c r="P52" s="126"/>
       <c r="S52" s="15"/>
       <c r="U52" s="59"/>
       <c r="V52" s="36"/>
-      <c r="W52" s="195"/>
-      <c r="X52" s="196"/>
-      <c r="Y52" s="196"/>
-      <c r="Z52" s="196"/>
-      <c r="AA52" s="196"/>
-      <c r="AB52" s="196"/>
-      <c r="AC52" s="196"/>
-      <c r="AD52" s="196"/>
-      <c r="AE52" s="196"/>
-      <c r="AF52" s="196"/>
-      <c r="AG52" s="196"/>
-      <c r="AH52" s="196"/>
-      <c r="AI52" s="196"/>
-      <c r="AJ52" s="197"/>
+      <c r="W52" s="163"/>
+      <c r="X52" s="164"/>
+      <c r="Y52" s="164"/>
+      <c r="Z52" s="164"/>
+      <c r="AA52" s="164"/>
+      <c r="AB52" s="164"/>
+      <c r="AC52" s="164"/>
+      <c r="AD52" s="164"/>
+      <c r="AE52" s="164"/>
+      <c r="AF52" s="164"/>
+      <c r="AG52" s="164"/>
+      <c r="AH52" s="164"/>
+      <c r="AI52" s="164"/>
+      <c r="AJ52" s="165"/>
       <c r="AK52" s="23"/>
       <c r="AL52" s="21"/>
       <c r="AM52" s="23"/>
@@ -7249,35 +7196,35 @@
       <c r="C53" s="16"/>
       <c r="D53" s="2"/>
       <c r="E53" s="52"/>
-      <c r="F53" s="202"/>
-      <c r="G53" s="202"/>
-      <c r="H53" s="202"/>
-      <c r="I53" s="202"/>
+      <c r="F53" s="126"/>
+      <c r="G53" s="126"/>
+      <c r="H53" s="126"/>
+      <c r="I53" s="126"/>
       <c r="J53" s="52"/>
       <c r="K53" s="52"/>
       <c r="L53" s="52"/>
-      <c r="M53" s="202"/>
-      <c r="N53" s="202"/>
-      <c r="O53" s="202"/>
-      <c r="P53" s="202"/>
+      <c r="M53" s="126"/>
+      <c r="N53" s="126"/>
+      <c r="O53" s="126"/>
+      <c r="P53" s="126"/>
       <c r="Q53" s="52"/>
       <c r="S53" s="15"/>
       <c r="U53" s="59"/>
       <c r="V53" s="35"/>
-      <c r="W53" s="198"/>
-      <c r="X53" s="199"/>
-      <c r="Y53" s="199"/>
-      <c r="Z53" s="199"/>
-      <c r="AA53" s="199"/>
-      <c r="AB53" s="199"/>
-      <c r="AC53" s="199"/>
-      <c r="AD53" s="199"/>
-      <c r="AE53" s="199"/>
-      <c r="AF53" s="199"/>
-      <c r="AG53" s="199"/>
-      <c r="AH53" s="199"/>
-      <c r="AI53" s="199"/>
-      <c r="AJ53" s="200"/>
+      <c r="W53" s="166"/>
+      <c r="X53" s="167"/>
+      <c r="Y53" s="167"/>
+      <c r="Z53" s="167"/>
+      <c r="AA53" s="167"/>
+      <c r="AB53" s="167"/>
+      <c r="AC53" s="167"/>
+      <c r="AD53" s="167"/>
+      <c r="AE53" s="167"/>
+      <c r="AF53" s="167"/>
+      <c r="AG53" s="167"/>
+      <c r="AH53" s="167"/>
+      <c r="AI53" s="167"/>
+      <c r="AJ53" s="168"/>
       <c r="AK53" s="16"/>
       <c r="AL53" s="15"/>
       <c r="AM53" s="16"/>
@@ -7307,20 +7254,20 @@
       <c r="S54" s="15"/>
       <c r="U54" s="16"/>
       <c r="V54" s="34"/>
-      <c r="W54" s="192"/>
-      <c r="X54" s="193"/>
-      <c r="Y54" s="193"/>
-      <c r="Z54" s="193"/>
-      <c r="AA54" s="193"/>
-      <c r="AB54" s="193"/>
-      <c r="AC54" s="193"/>
-      <c r="AD54" s="193"/>
-      <c r="AE54" s="193"/>
-      <c r="AF54" s="193"/>
-      <c r="AG54" s="193"/>
-      <c r="AH54" s="193"/>
-      <c r="AI54" s="193"/>
-      <c r="AJ54" s="194"/>
+      <c r="W54" s="151"/>
+      <c r="X54" s="152"/>
+      <c r="Y54" s="152"/>
+      <c r="Z54" s="152"/>
+      <c r="AA54" s="152"/>
+      <c r="AB54" s="152"/>
+      <c r="AC54" s="152"/>
+      <c r="AD54" s="152"/>
+      <c r="AE54" s="152"/>
+      <c r="AF54" s="152"/>
+      <c r="AG54" s="152"/>
+      <c r="AH54" s="152"/>
+      <c r="AI54" s="152"/>
+      <c r="AJ54" s="153"/>
       <c r="AK54" s="11"/>
       <c r="AL54" s="9"/>
       <c r="AM54" s="11"/>
@@ -7468,39 +7415,39 @@
       <c r="G59" s="28"/>
       <c r="S59" s="15"/>
       <c r="U59" s="16"/>
-      <c r="V59" s="136" t="s">
+      <c r="V59" s="123" t="s">
         <v>23</v>
       </c>
-      <c r="W59" s="152" t="s">
+      <c r="W59" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="X59" s="156"/>
-      <c r="Y59" s="156"/>
-      <c r="Z59" s="156"/>
-      <c r="AA59" s="156"/>
-      <c r="AB59" s="156"/>
-      <c r="AC59" s="156"/>
-      <c r="AD59" s="156"/>
-      <c r="AE59" s="156"/>
-      <c r="AF59" s="156"/>
-      <c r="AG59" s="156"/>
-      <c r="AH59" s="156"/>
-      <c r="AI59" s="156"/>
-      <c r="AJ59" s="153"/>
-      <c r="AK59" s="152" t="s">
+      <c r="X59" s="137"/>
+      <c r="Y59" s="137"/>
+      <c r="Z59" s="137"/>
+      <c r="AA59" s="137"/>
+      <c r="AB59" s="137"/>
+      <c r="AC59" s="137"/>
+      <c r="AD59" s="137"/>
+      <c r="AE59" s="137"/>
+      <c r="AF59" s="137"/>
+      <c r="AG59" s="137"/>
+      <c r="AH59" s="137"/>
+      <c r="AI59" s="137"/>
+      <c r="AJ59" s="134"/>
+      <c r="AK59" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="AL59" s="153"/>
-      <c r="AM59" s="152" t="s">
+      <c r="AL59" s="134"/>
+      <c r="AM59" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="AN59" s="156"/>
-      <c r="AO59" s="153"/>
-      <c r="AP59" s="158" t="s">
+      <c r="AN59" s="137"/>
+      <c r="AO59" s="134"/>
+      <c r="AP59" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="AQ59" s="159"/>
-      <c r="AR59" s="160"/>
+      <c r="AQ59" s="128"/>
+      <c r="AR59" s="129"/>
       <c r="AS59" s="37"/>
       <c r="AT59" s="8"/>
     </row>
@@ -7517,29 +7464,29 @@
       <c r="G60" s="28"/>
       <c r="S60" s="15"/>
       <c r="U60" s="16"/>
-      <c r="V60" s="137"/>
-      <c r="W60" s="154"/>
-      <c r="X60" s="157"/>
-      <c r="Y60" s="157"/>
-      <c r="Z60" s="157"/>
-      <c r="AA60" s="157"/>
-      <c r="AB60" s="157"/>
-      <c r="AC60" s="157"/>
-      <c r="AD60" s="157"/>
-      <c r="AE60" s="157"/>
-      <c r="AF60" s="157"/>
-      <c r="AG60" s="157"/>
-      <c r="AH60" s="157"/>
-      <c r="AI60" s="157"/>
-      <c r="AJ60" s="155"/>
-      <c r="AK60" s="154"/>
-      <c r="AL60" s="155"/>
-      <c r="AM60" s="154"/>
-      <c r="AN60" s="157"/>
-      <c r="AO60" s="155"/>
-      <c r="AP60" s="161"/>
-      <c r="AQ60" s="162"/>
-      <c r="AR60" s="163"/>
+      <c r="V60" s="124"/>
+      <c r="W60" s="135"/>
+      <c r="X60" s="138"/>
+      <c r="Y60" s="138"/>
+      <c r="Z60" s="138"/>
+      <c r="AA60" s="138"/>
+      <c r="AB60" s="138"/>
+      <c r="AC60" s="138"/>
+      <c r="AD60" s="138"/>
+      <c r="AE60" s="138"/>
+      <c r="AF60" s="138"/>
+      <c r="AG60" s="138"/>
+      <c r="AH60" s="138"/>
+      <c r="AI60" s="138"/>
+      <c r="AJ60" s="136"/>
+      <c r="AK60" s="135"/>
+      <c r="AL60" s="136"/>
+      <c r="AM60" s="135"/>
+      <c r="AN60" s="138"/>
+      <c r="AO60" s="136"/>
+      <c r="AP60" s="130"/>
+      <c r="AQ60" s="131"/>
+      <c r="AR60" s="132"/>
       <c r="AS60" s="37"/>
       <c r="AT60" s="8"/>
     </row>
@@ -7558,20 +7505,20 @@
       <c r="S61" s="15"/>
       <c r="U61" s="16"/>
       <c r="V61" s="51"/>
-      <c r="W61" s="164"/>
-      <c r="X61" s="165"/>
-      <c r="Y61" s="165"/>
-      <c r="Z61" s="165"/>
-      <c r="AA61" s="165"/>
-      <c r="AB61" s="165"/>
-      <c r="AC61" s="165"/>
-      <c r="AD61" s="165"/>
-      <c r="AE61" s="165"/>
-      <c r="AF61" s="165"/>
-      <c r="AG61" s="165"/>
-      <c r="AH61" s="165"/>
-      <c r="AI61" s="165"/>
-      <c r="AJ61" s="166"/>
+      <c r="W61" s="154"/>
+      <c r="X61" s="155"/>
+      <c r="Y61" s="155"/>
+      <c r="Z61" s="155"/>
+      <c r="AA61" s="155"/>
+      <c r="AB61" s="155"/>
+      <c r="AC61" s="155"/>
+      <c r="AD61" s="155"/>
+      <c r="AE61" s="155"/>
+      <c r="AF61" s="155"/>
+      <c r="AG61" s="155"/>
+      <c r="AH61" s="155"/>
+      <c r="AI61" s="155"/>
+      <c r="AJ61" s="156"/>
       <c r="AK61" s="47"/>
       <c r="AL61" s="45"/>
       <c r="AM61" s="47"/>
@@ -7598,20 +7545,20 @@
       <c r="S62" s="15"/>
       <c r="U62" s="16"/>
       <c r="V62" s="43"/>
-      <c r="W62" s="167"/>
-      <c r="X62" s="168"/>
-      <c r="Y62" s="168"/>
-      <c r="Z62" s="168"/>
-      <c r="AA62" s="168"/>
-      <c r="AB62" s="168"/>
-      <c r="AC62" s="168"/>
-      <c r="AD62" s="168"/>
-      <c r="AE62" s="168"/>
-      <c r="AF62" s="168"/>
-      <c r="AG62" s="168"/>
-      <c r="AH62" s="168"/>
-      <c r="AI62" s="168"/>
-      <c r="AJ62" s="169"/>
+      <c r="W62" s="157"/>
+      <c r="X62" s="158"/>
+      <c r="Y62" s="158"/>
+      <c r="Z62" s="158"/>
+      <c r="AA62" s="158"/>
+      <c r="AB62" s="158"/>
+      <c r="AC62" s="158"/>
+      <c r="AD62" s="158"/>
+      <c r="AE62" s="158"/>
+      <c r="AF62" s="158"/>
+      <c r="AG62" s="158"/>
+      <c r="AH62" s="158"/>
+      <c r="AI62" s="158"/>
+      <c r="AJ62" s="159"/>
       <c r="AK62" s="39"/>
       <c r="AL62" s="38"/>
       <c r="AM62" s="39"/>
@@ -7633,20 +7580,20 @@
       <c r="S63" s="15"/>
       <c r="U63" s="16"/>
       <c r="V63" s="34"/>
-      <c r="W63" s="170"/>
-      <c r="X63" s="171"/>
-      <c r="Y63" s="171"/>
-      <c r="Z63" s="171"/>
-      <c r="AA63" s="171"/>
-      <c r="AB63" s="171"/>
-      <c r="AC63" s="171"/>
-      <c r="AD63" s="171"/>
-      <c r="AE63" s="171"/>
-      <c r="AF63" s="171"/>
-      <c r="AG63" s="171"/>
-      <c r="AH63" s="171"/>
-      <c r="AI63" s="171"/>
-      <c r="AJ63" s="172"/>
+      <c r="W63" s="160"/>
+      <c r="X63" s="161"/>
+      <c r="Y63" s="161"/>
+      <c r="Z63" s="161"/>
+      <c r="AA63" s="161"/>
+      <c r="AB63" s="161"/>
+      <c r="AC63" s="161"/>
+      <c r="AD63" s="161"/>
+      <c r="AE63" s="161"/>
+      <c r="AF63" s="161"/>
+      <c r="AG63" s="161"/>
+      <c r="AH63" s="161"/>
+      <c r="AI63" s="161"/>
+      <c r="AJ63" s="162"/>
       <c r="AK63" s="11"/>
       <c r="AL63" s="9"/>
       <c r="AM63" s="11"/>
@@ -7661,28 +7608,28 @@
     <row r="64" spans="2:46" ht="25.05" customHeight="1">
       <c r="B64" s="14"/>
       <c r="C64" s="20"/>
-      <c r="D64" s="201"/>
-      <c r="E64" s="201"/>
-      <c r="F64" s="201"/>
-      <c r="G64" s="201"/>
+      <c r="D64" s="125"/>
+      <c r="E64" s="125"/>
+      <c r="F64" s="125"/>
+      <c r="G64" s="125"/>
       <c r="N64" s="2"/>
       <c r="S64" s="15"/>
       <c r="U64" s="16"/>
       <c r="V64" s="36"/>
-      <c r="W64" s="195"/>
-      <c r="X64" s="196"/>
-      <c r="Y64" s="196"/>
-      <c r="Z64" s="196"/>
-      <c r="AA64" s="196"/>
-      <c r="AB64" s="196"/>
-      <c r="AC64" s="196"/>
-      <c r="AD64" s="196"/>
-      <c r="AE64" s="196"/>
-      <c r="AF64" s="196"/>
-      <c r="AG64" s="196"/>
-      <c r="AH64" s="196"/>
-      <c r="AI64" s="196"/>
-      <c r="AJ64" s="197"/>
+      <c r="W64" s="163"/>
+      <c r="X64" s="164"/>
+      <c r="Y64" s="164"/>
+      <c r="Z64" s="164"/>
+      <c r="AA64" s="164"/>
+      <c r="AB64" s="164"/>
+      <c r="AC64" s="164"/>
+      <c r="AD64" s="164"/>
+      <c r="AE64" s="164"/>
+      <c r="AF64" s="164"/>
+      <c r="AG64" s="164"/>
+      <c r="AH64" s="164"/>
+      <c r="AI64" s="164"/>
+      <c r="AJ64" s="165"/>
       <c r="AK64" s="23"/>
       <c r="AL64" s="21"/>
       <c r="AM64" s="23"/>
@@ -7704,20 +7651,20 @@
       <c r="S65" s="15"/>
       <c r="U65" s="16"/>
       <c r="V65" s="35"/>
-      <c r="W65" s="198"/>
-      <c r="X65" s="199"/>
-      <c r="Y65" s="199"/>
-      <c r="Z65" s="199"/>
-      <c r="AA65" s="199"/>
-      <c r="AB65" s="199"/>
-      <c r="AC65" s="199"/>
-      <c r="AD65" s="199"/>
-      <c r="AE65" s="199"/>
-      <c r="AF65" s="199"/>
-      <c r="AG65" s="199"/>
-      <c r="AH65" s="199"/>
-      <c r="AI65" s="199"/>
-      <c r="AJ65" s="200"/>
+      <c r="W65" s="166"/>
+      <c r="X65" s="167"/>
+      <c r="Y65" s="167"/>
+      <c r="Z65" s="167"/>
+      <c r="AA65" s="167"/>
+      <c r="AB65" s="167"/>
+      <c r="AC65" s="167"/>
+      <c r="AD65" s="167"/>
+      <c r="AE65" s="167"/>
+      <c r="AF65" s="167"/>
+      <c r="AG65" s="167"/>
+      <c r="AH65" s="167"/>
+      <c r="AI65" s="167"/>
+      <c r="AJ65" s="168"/>
       <c r="AK65" s="16"/>
       <c r="AL65" s="15"/>
       <c r="AM65" s="16"/>
@@ -7737,20 +7684,20 @@
       <c r="S66" s="15"/>
       <c r="U66" s="16"/>
       <c r="V66" s="34"/>
-      <c r="W66" s="192"/>
-      <c r="X66" s="193"/>
-      <c r="Y66" s="193"/>
-      <c r="Z66" s="193"/>
-      <c r="AA66" s="193"/>
-      <c r="AB66" s="193"/>
-      <c r="AC66" s="193"/>
-      <c r="AD66" s="193"/>
-      <c r="AE66" s="193"/>
-      <c r="AF66" s="193"/>
-      <c r="AG66" s="193"/>
-      <c r="AH66" s="193"/>
-      <c r="AI66" s="193"/>
-      <c r="AJ66" s="194"/>
+      <c r="W66" s="151"/>
+      <c r="X66" s="152"/>
+      <c r="Y66" s="152"/>
+      <c r="Z66" s="152"/>
+      <c r="AA66" s="152"/>
+      <c r="AB66" s="152"/>
+      <c r="AC66" s="152"/>
+      <c r="AD66" s="152"/>
+      <c r="AE66" s="152"/>
+      <c r="AF66" s="152"/>
+      <c r="AG66" s="152"/>
+      <c r="AH66" s="152"/>
+      <c r="AI66" s="152"/>
+      <c r="AJ66" s="153"/>
       <c r="AK66" s="11"/>
       <c r="AL66" s="9"/>
       <c r="AM66" s="11"/>
@@ -7934,11 +7881,11 @@
       <c r="AE73" s="22"/>
       <c r="AF73" s="22"/>
       <c r="AG73" s="21"/>
-      <c r="AI73" s="183"/>
-      <c r="AJ73" s="184"/>
-      <c r="AK73" s="184"/>
-      <c r="AL73" s="184"/>
-      <c r="AM73" s="184"/>
+      <c r="AI73" s="142"/>
+      <c r="AJ73" s="143"/>
+      <c r="AK73" s="143"/>
+      <c r="AL73" s="143"/>
+      <c r="AM73" s="143"/>
       <c r="AN73" s="23" t="s">
         <v>5</v>
       </c>
@@ -7965,11 +7912,11 @@
       <c r="AE74" s="10"/>
       <c r="AF74" s="10"/>
       <c r="AG74" s="9"/>
-      <c r="AI74" s="185"/>
-      <c r="AJ74" s="186"/>
-      <c r="AK74" s="186"/>
-      <c r="AL74" s="186"/>
-      <c r="AM74" s="186"/>
+      <c r="AI74" s="144"/>
+      <c r="AJ74" s="145"/>
+      <c r="AK74" s="145"/>
+      <c r="AL74" s="145"/>
+      <c r="AM74" s="145"/>
       <c r="AN74" s="16"/>
       <c r="AR74" s="15"/>
       <c r="AT74" s="8"/>
@@ -7993,30 +7940,30 @@
       <c r="Q75" s="10"/>
       <c r="R75" s="10"/>
       <c r="S75" s="9"/>
-      <c r="U75" s="189" t="s">
+      <c r="U75" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="V75" s="190"/>
-      <c r="W75" s="190"/>
-      <c r="X75" s="191"/>
-      <c r="Y75" s="189" t="s">
+      <c r="V75" s="149"/>
+      <c r="W75" s="149"/>
+      <c r="X75" s="150"/>
+      <c r="Y75" s="148" t="s">
         <v>3</v>
       </c>
-      <c r="Z75" s="190"/>
-      <c r="AA75" s="190"/>
-      <c r="AB75" s="190"/>
-      <c r="AC75" s="190"/>
-      <c r="AD75" s="192" t="s">
+      <c r="Z75" s="149"/>
+      <c r="AA75" s="149"/>
+      <c r="AB75" s="149"/>
+      <c r="AC75" s="149"/>
+      <c r="AD75" s="151" t="s">
         <v>2</v>
       </c>
-      <c r="AE75" s="193"/>
-      <c r="AF75" s="193"/>
-      <c r="AG75" s="194"/>
-      <c r="AI75" s="187"/>
-      <c r="AJ75" s="188"/>
-      <c r="AK75" s="188"/>
-      <c r="AL75" s="188"/>
-      <c r="AM75" s="188"/>
+      <c r="AE75" s="152"/>
+      <c r="AF75" s="152"/>
+      <c r="AG75" s="153"/>
+      <c r="AI75" s="146"/>
+      <c r="AJ75" s="147"/>
+      <c r="AK75" s="147"/>
+      <c r="AL75" s="147"/>
+      <c r="AM75" s="147"/>
       <c r="AN75" s="11"/>
       <c r="AO75" s="10"/>
       <c r="AP75" s="10"/>
@@ -8132,21 +8079,27 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="V59:V60"/>
-    <mergeCell ref="D64:G64"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="M52:P52"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="M53:P53"/>
-    <mergeCell ref="AP59:AR60"/>
-    <mergeCell ref="AK17:AL18"/>
-    <mergeCell ref="AM17:AO18"/>
-    <mergeCell ref="AP17:AR18"/>
-    <mergeCell ref="AM47:AO48"/>
-    <mergeCell ref="AP47:AR48"/>
-    <mergeCell ref="AK59:AL60"/>
-    <mergeCell ref="AM59:AO60"/>
-    <mergeCell ref="AK47:AL48"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AO3:AT3"/>
+    <mergeCell ref="AO4:AQ5"/>
+    <mergeCell ref="L41:O42"/>
+    <mergeCell ref="P41:S42"/>
+    <mergeCell ref="V29:V30"/>
+    <mergeCell ref="AG2:AJ2"/>
+    <mergeCell ref="AK2:AN2"/>
+    <mergeCell ref="AO6:AT7"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="AG7:AJ7"/>
+    <mergeCell ref="AK7:AN7"/>
+    <mergeCell ref="L40:O40"/>
+    <mergeCell ref="P40:S40"/>
+    <mergeCell ref="W17:AJ18"/>
+    <mergeCell ref="J2:AB4"/>
+    <mergeCell ref="V47:V48"/>
+    <mergeCell ref="AK29:AL30"/>
+    <mergeCell ref="AM29:AO30"/>
+    <mergeCell ref="AP29:AR30"/>
+    <mergeCell ref="W31:AJ33"/>
     <mergeCell ref="AC2:AF2"/>
     <mergeCell ref="AI73:AM75"/>
     <mergeCell ref="U75:X75"/>
@@ -8163,27 +8116,21 @@
     <mergeCell ref="V17:V18"/>
     <mergeCell ref="W52:AJ54"/>
     <mergeCell ref="W59:AJ60"/>
-    <mergeCell ref="V47:V48"/>
-    <mergeCell ref="AK29:AL30"/>
-    <mergeCell ref="AM29:AO30"/>
-    <mergeCell ref="AP29:AR30"/>
-    <mergeCell ref="W31:AJ33"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AO3:AT3"/>
-    <mergeCell ref="AO4:AQ5"/>
-    <mergeCell ref="L41:O42"/>
-    <mergeCell ref="P41:S42"/>
-    <mergeCell ref="V29:V30"/>
-    <mergeCell ref="AG2:AJ2"/>
-    <mergeCell ref="AK2:AN2"/>
-    <mergeCell ref="AO6:AT7"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="AG7:AJ7"/>
-    <mergeCell ref="AK7:AN7"/>
-    <mergeCell ref="L40:O40"/>
-    <mergeCell ref="P40:S40"/>
-    <mergeCell ref="W17:AJ18"/>
-    <mergeCell ref="J2:AB4"/>
+    <mergeCell ref="AP59:AR60"/>
+    <mergeCell ref="AK17:AL18"/>
+    <mergeCell ref="AM17:AO18"/>
+    <mergeCell ref="AP17:AR18"/>
+    <mergeCell ref="AM47:AO48"/>
+    <mergeCell ref="AP47:AR48"/>
+    <mergeCell ref="AK59:AL60"/>
+    <mergeCell ref="AM59:AO60"/>
+    <mergeCell ref="AK47:AL48"/>
+    <mergeCell ref="V59:V60"/>
+    <mergeCell ref="D64:G64"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="M52:P52"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="M53:P53"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>

</xml_diff>